<commit_message>
Issue #12 Actualizo casos de prueba por Sprint 2
</commit_message>
<xml_diff>
--- a/testing/Casos de prueba - G7.xlsx
+++ b/testing/Casos de prueba - G7.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="234">
   <si>
     <t>Proyecto</t>
   </si>
@@ -430,6 +430,18 @@
   </si>
   <si>
     <t>Valida que el usuario existe. Muestra mensaje con motivo de rechazo.</t>
+  </si>
+  <si>
+    <t>PI-S1-0015</t>
+  </si>
+  <si>
+    <t>PI-S1-0016</t>
+  </si>
+  <si>
+    <t>PI-S1-0017</t>
+  </si>
+  <si>
+    <t>PI-S1-0018</t>
   </si>
   <si>
     <t>Método</t>
@@ -951,7 +963,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1099,6 +1111,8 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
@@ -1466,7 +1480,7 @@
       </c>
       <c r="C4" s="6">
         <f>TODAY()</f>
-        <v>44861</v>
+        <v>44869</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
@@ -2738,7 +2752,9 @@
     </row>
     <row r="45">
       <c r="A45" s="48"/>
-      <c r="B45" s="49"/>
+      <c r="B45" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="C45" s="49"/>
       <c r="D45" s="50"/>
       <c r="E45" s="49"/>
@@ -2756,7 +2772,7 @@
     </row>
     <row r="46">
       <c r="A46" s="48"/>
-      <c r="B46" s="49"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="49"/>
       <c r="D46" s="50"/>
       <c r="E46" s="49"/>
@@ -2774,7 +2790,7 @@
     </row>
     <row r="47">
       <c r="A47" s="48"/>
-      <c r="B47" s="49"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="49"/>
       <c r="D47" s="50"/>
       <c r="E47" s="49"/>
@@ -2792,7 +2808,7 @@
     </row>
     <row r="48">
       <c r="A48" s="48"/>
-      <c r="B48" s="49"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="49"/>
       <c r="D48" s="50"/>
       <c r="E48" s="49"/>
@@ -2810,7 +2826,7 @@
     </row>
     <row r="49">
       <c r="A49" s="48"/>
-      <c r="B49" s="49"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="49"/>
       <c r="D49" s="50"/>
       <c r="E49" s="49"/>
@@ -2828,7 +2844,7 @@
     </row>
     <row r="50">
       <c r="A50" s="48"/>
-      <c r="B50" s="49"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="49"/>
       <c r="D50" s="50"/>
       <c r="E50" s="49"/>
@@ -2846,7 +2862,9 @@
     </row>
     <row r="51">
       <c r="A51" s="48"/>
-      <c r="B51" s="49"/>
+      <c r="B51" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="C51" s="49"/>
       <c r="D51" s="50"/>
       <c r="E51" s="49"/>
@@ -2864,7 +2882,7 @@
     </row>
     <row r="52">
       <c r="A52" s="48"/>
-      <c r="B52" s="49"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="49"/>
       <c r="D52" s="50"/>
       <c r="E52" s="49"/>
@@ -2882,7 +2900,7 @@
     </row>
     <row r="53">
       <c r="A53" s="48"/>
-      <c r="B53" s="49"/>
+      <c r="B53" s="55"/>
       <c r="C53" s="49"/>
       <c r="D53" s="50"/>
       <c r="E53" s="49"/>
@@ -2900,7 +2918,7 @@
     </row>
     <row r="54">
       <c r="A54" s="48"/>
-      <c r="B54" s="49"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="49"/>
       <c r="D54" s="50"/>
       <c r="E54" s="49"/>
@@ -2918,7 +2936,7 @@
     </row>
     <row r="55">
       <c r="A55" s="48"/>
-      <c r="B55" s="49"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="49"/>
       <c r="D55" s="50"/>
       <c r="E55" s="49"/>
@@ -2936,7 +2954,7 @@
     </row>
     <row r="56">
       <c r="A56" s="48"/>
-      <c r="B56" s="49"/>
+      <c r="B56" s="56"/>
       <c r="C56" s="49"/>
       <c r="D56" s="50"/>
       <c r="E56" s="49"/>
@@ -2954,7 +2972,9 @@
     </row>
     <row r="57">
       <c r="A57" s="48"/>
-      <c r="B57" s="49"/>
+      <c r="B57" s="21" t="s">
+        <v>133</v>
+      </c>
       <c r="C57" s="49"/>
       <c r="D57" s="50"/>
       <c r="E57" s="49"/>
@@ -2972,7 +2992,7 @@
     </row>
     <row r="58">
       <c r="A58" s="48"/>
-      <c r="B58" s="49"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="49"/>
       <c r="D58" s="50"/>
       <c r="E58" s="49"/>
@@ -2990,7 +3010,7 @@
     </row>
     <row r="59">
       <c r="A59" s="48"/>
-      <c r="B59" s="49"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="49"/>
       <c r="D59" s="50"/>
       <c r="E59" s="49"/>
@@ -3008,7 +3028,7 @@
     </row>
     <row r="60">
       <c r="A60" s="48"/>
-      <c r="B60" s="49"/>
+      <c r="B60" s="55"/>
       <c r="C60" s="49"/>
       <c r="D60" s="50"/>
       <c r="E60" s="49"/>
@@ -3026,7 +3046,7 @@
     </row>
     <row r="61">
       <c r="A61" s="48"/>
-      <c r="B61" s="49"/>
+      <c r="B61" s="55"/>
       <c r="C61" s="49"/>
       <c r="D61" s="50"/>
       <c r="E61" s="49"/>
@@ -3044,7 +3064,7 @@
     </row>
     <row r="62">
       <c r="A62" s="48"/>
-      <c r="B62" s="49"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="49"/>
       <c r="D62" s="50"/>
       <c r="E62" s="49"/>
@@ -3062,7 +3082,9 @@
     </row>
     <row r="63">
       <c r="A63" s="48"/>
-      <c r="B63" s="49"/>
+      <c r="B63" s="21" t="s">
+        <v>134</v>
+      </c>
       <c r="C63" s="49"/>
       <c r="D63" s="50"/>
       <c r="E63" s="49"/>
@@ -3080,7 +3102,7 @@
     </row>
     <row r="64">
       <c r="A64" s="48"/>
-      <c r="B64" s="49"/>
+      <c r="B64" s="55"/>
       <c r="C64" s="49"/>
       <c r="D64" s="50"/>
       <c r="E64" s="49"/>
@@ -3098,7 +3120,7 @@
     </row>
     <row r="65">
       <c r="A65" s="48"/>
-      <c r="B65" s="49"/>
+      <c r="B65" s="55"/>
       <c r="C65" s="49"/>
       <c r="D65" s="50"/>
       <c r="E65" s="49"/>
@@ -3116,7 +3138,7 @@
     </row>
     <row r="66">
       <c r="A66" s="48"/>
-      <c r="B66" s="49"/>
+      <c r="B66" s="55"/>
       <c r="C66" s="49"/>
       <c r="D66" s="50"/>
       <c r="E66" s="49"/>
@@ -3134,7 +3156,7 @@
     </row>
     <row r="67">
       <c r="A67" s="48"/>
-      <c r="B67" s="49"/>
+      <c r="B67" s="55"/>
       <c r="C67" s="49"/>
       <c r="D67" s="50"/>
       <c r="E67" s="49"/>
@@ -3152,7 +3174,7 @@
     </row>
     <row r="68">
       <c r="A68" s="48"/>
-      <c r="B68" s="49"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="49"/>
       <c r="D68" s="50"/>
       <c r="E68" s="49"/>
@@ -19549,104 +19571,108 @@
       <c r="P978" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="97">
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="K28:K31"/>
+  <mergeCells count="101">
+    <mergeCell ref="L14:L19"/>
+    <mergeCell ref="M14:M19"/>
+    <mergeCell ref="N14:N19"/>
+    <mergeCell ref="O14:O19"/>
+    <mergeCell ref="P14:P19"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="I14:I19"/>
+    <mergeCell ref="J14:J19"/>
+    <mergeCell ref="K14:K19"/>
+    <mergeCell ref="L24:L27"/>
+    <mergeCell ref="M24:M27"/>
+    <mergeCell ref="N24:N27"/>
+    <mergeCell ref="O24:O27"/>
+    <mergeCell ref="P24:P27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="K24:K27"/>
     <mergeCell ref="L28:L31"/>
-    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="M28:M31"/>
+    <mergeCell ref="N28:N31"/>
+    <mergeCell ref="O28:O31"/>
+    <mergeCell ref="P28:P31"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="E28:E31"/>
-    <mergeCell ref="N28:N31"/>
-    <mergeCell ref="O28:O31"/>
-    <mergeCell ref="M28:M31"/>
-    <mergeCell ref="P28:P31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="L33:L38"/>
+    <mergeCell ref="M33:M38"/>
+    <mergeCell ref="N33:N38"/>
+    <mergeCell ref="O33:O38"/>
     <mergeCell ref="P33:P38"/>
-    <mergeCell ref="P24:P27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J33:J38"/>
-    <mergeCell ref="K33:K38"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="N24:N27"/>
-    <mergeCell ref="O24:O27"/>
-    <mergeCell ref="M24:M27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="L24:L27"/>
-    <mergeCell ref="L33:L38"/>
-    <mergeCell ref="I33:I38"/>
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="C33:C38"/>
     <mergeCell ref="D33:D38"/>
     <mergeCell ref="E33:E38"/>
-    <mergeCell ref="N33:N38"/>
-    <mergeCell ref="O33:O38"/>
-    <mergeCell ref="M33:M38"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="I33:I38"/>
+    <mergeCell ref="J33:J38"/>
+    <mergeCell ref="K33:K38"/>
+    <mergeCell ref="L39:L44"/>
+    <mergeCell ref="M39:M44"/>
+    <mergeCell ref="N39:N44"/>
+    <mergeCell ref="O39:O44"/>
+    <mergeCell ref="P39:P44"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="I39:I44"/>
+    <mergeCell ref="J39:J44"/>
+    <mergeCell ref="K39:K44"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:H6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P39:P44"/>
-    <mergeCell ref="J39:J44"/>
-    <mergeCell ref="K39:K44"/>
-    <mergeCell ref="L39:L44"/>
-    <mergeCell ref="I39:I44"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="N39:N44"/>
-    <mergeCell ref="O39:O44"/>
-    <mergeCell ref="M39:M44"/>
-    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="M11:M12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I14:I19"/>
-    <mergeCell ref="J14:J19"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="P14:P19"/>
-    <mergeCell ref="K14:K19"/>
-    <mergeCell ref="L14:L19"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="N14:N19"/>
-    <mergeCell ref="O14:O19"/>
-    <mergeCell ref="M14:M19"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="B63:B68"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="J8:J9 J11 J13:J14 J20:J24 J28 J32:J33 J39">
@@ -19722,7 +19748,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="55"/>
+      <c r="S1" s="57"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -19747,7 +19773,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="56"/>
+      <c r="S2" s="58"/>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
@@ -19772,7 +19798,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="57"/>
+      <c r="S3" s="59"/>
     </row>
     <row r="4">
       <c r="A4" s="1"/>
@@ -19781,7 +19807,7 @@
       </c>
       <c r="C4" s="6">
         <f>TODAY()</f>
-        <v>44861</v>
+        <v>44869</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
@@ -19798,7 +19824,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="56"/>
+      <c r="S4" s="58"/>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
@@ -19819,7 +19845,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-      <c r="S5" s="57"/>
+      <c r="S5" s="59"/>
     </row>
     <row r="6">
       <c r="A6" s="1"/>
@@ -19836,7 +19862,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>8</v>
@@ -19847,16 +19873,16 @@
         <v>9</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L6" s="58" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>137</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>12</v>
@@ -19870,7 +19896,7 @@
       <c r="R6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S6" s="56"/>
+      <c r="S6" s="58"/>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
@@ -19897,48 +19923,48 @@
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
-      <c r="S7" s="57"/>
+      <c r="S7" s="59"/>
     </row>
     <row r="8">
       <c r="A8" s="16"/>
       <c r="B8" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="59">
+        <v>144</v>
+      </c>
+      <c r="G8" s="61">
         <v>1.0</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K8" s="17">
         <v>200.0</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="O8" s="17" t="s">
         <v>28</v>
@@ -19949,46 +19975,46 @@
       <c r="Q8" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R8" s="60">
+      <c r="R8" s="62">
         <f t="shared" ref="R8:R10" si="1">today()</f>
-        <v>44861</v>
-      </c>
-      <c r="S8" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S8" s="63"/>
     </row>
     <row r="9">
-      <c r="A9" s="62"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="21" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G9" s="21">
         <v>1.0</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="K9" s="21">
         <v>200.0</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
@@ -20001,46 +20027,46 @@
       <c r="Q9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="63">
+      <c r="R9" s="65">
         <f t="shared" si="1"/>
-        <v>44861</v>
-      </c>
-      <c r="S9" s="64"/>
+        <v>44869</v>
+      </c>
+      <c r="S9" s="66"/>
     </row>
     <row r="10" ht="47.25" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="17" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="G10" s="59">
+        <v>163</v>
+      </c>
+      <c r="G10" s="61">
         <v>1.0</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K10" s="17">
         <v>200.0</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
@@ -20053,11 +20079,11 @@
       <c r="Q10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R10" s="60">
+      <c r="R10" s="62">
         <f t="shared" si="1"/>
-        <v>44861</v>
-      </c>
-      <c r="S10" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S10" s="63"/>
     </row>
     <row r="11">
       <c r="A11" s="48"/>
@@ -20066,11 +20092,11 @@
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
-      <c r="G11" s="59">
+      <c r="G11" s="61">
         <v>2.0</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
@@ -20082,42 +20108,42 @@
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
-      <c r="S11" s="65"/>
+      <c r="S11" s="67"/>
     </row>
     <row r="12">
       <c r="A12" s="48"/>
       <c r="B12" s="21" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="G12" s="66">
+        <v>163</v>
+      </c>
+      <c r="G12" s="68">
         <v>1.0</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="K12" s="16">
         <v>409.0</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
@@ -20130,9 +20156,9 @@
       <c r="Q12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R12" s="63">
+      <c r="R12" s="65">
         <f>today()</f>
-        <v>44861</v>
+        <v>44869</v>
       </c>
       <c r="S12" s="48"/>
     </row>
@@ -20143,11 +20169,11 @@
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
-      <c r="G13" s="66">
+      <c r="G13" s="68">
         <v>2.0</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
@@ -20163,37 +20189,37 @@
     <row r="14" ht="47.25" customHeight="1">
       <c r="A14" s="16"/>
       <c r="B14" s="17" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" s="59">
+        <v>180</v>
+      </c>
+      <c r="G14" s="61">
         <v>1.0</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="K14" s="17">
         <v>200.0</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -20206,44 +20232,44 @@
       <c r="Q14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R14" s="60">
+      <c r="R14" s="62">
         <f t="shared" ref="R14:R16" si="2">today()</f>
-        <v>44861</v>
-      </c>
-      <c r="S14" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S14" s="63"/>
     </row>
     <row r="15" ht="47.25" customHeight="1">
       <c r="A15" s="16"/>
       <c r="B15" s="21" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="G15" s="66">
+        <v>180</v>
+      </c>
+      <c r="G15" s="68">
         <v>1.0</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="J15" s="22"/>
       <c r="K15" s="21">
         <v>204.0</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -20256,46 +20282,46 @@
       <c r="Q15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="63">
+      <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>44861</v>
-      </c>
-      <c r="S15" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S15" s="63"/>
     </row>
     <row r="16" ht="47.25" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G16" s="59">
+        <v>196</v>
+      </c>
+      <c r="G16" s="61">
         <v>1.0</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="K16" s="17">
         <v>200.0</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
@@ -20308,11 +20334,11 @@
       <c r="Q16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R16" s="60">
+      <c r="R16" s="62">
         <f t="shared" si="2"/>
-        <v>44861</v>
-      </c>
-      <c r="S16" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S16" s="63"/>
     </row>
     <row r="17">
       <c r="A17" s="16"/>
@@ -20321,11 +20347,11 @@
       <c r="D17" s="27"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="59">
+      <c r="G17" s="61">
         <v>2.0</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
@@ -20337,60 +20363,60 @@
       <c r="P17" s="27"/>
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
-      <c r="S17" s="61"/>
+      <c r="S17" s="63"/>
     </row>
     <row r="18">
-      <c r="A18" s="62"/>
-      <c r="B18" s="67" t="s">
-        <v>196</v>
-      </c>
-      <c r="C18" s="67" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18" s="67" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="67" t="s">
-        <v>199</v>
-      </c>
-      <c r="F18" s="67" t="s">
-        <v>140</v>
-      </c>
-      <c r="G18" s="67">
+      <c r="A18" s="64"/>
+      <c r="B18" s="69" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="E18" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="G18" s="69">
         <v>1.0</v>
       </c>
-      <c r="H18" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="I18" s="67" t="s">
-        <v>201</v>
-      </c>
-      <c r="J18" s="68"/>
-      <c r="K18" s="67">
+      <c r="H18" s="69" t="s">
+        <v>204</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>205</v>
+      </c>
+      <c r="J18" s="70"/>
+      <c r="K18" s="69">
         <v>204.0</v>
       </c>
-      <c r="L18" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="67" t="s">
+      <c r="L18" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="P18" s="67" t="s">
+      <c r="P18" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="Q18" s="67" t="s">
+      <c r="Q18" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="R18" s="69">
+      <c r="R18" s="71">
         <f>today()</f>
-        <v>44861</v>
-      </c>
-      <c r="S18" s="61"/>
+        <v>44869</v>
+      </c>
+      <c r="S18" s="63"/>
     </row>
     <row r="19">
-      <c r="A19" s="62"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -20399,7 +20425,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
-      <c r="J19" s="70"/>
+      <c r="J19" s="72"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -20408,10 +20434,10 @@
       <c r="P19" s="16"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
-      <c r="S19" s="64"/>
+      <c r="S19" s="66"/>
     </row>
     <row r="20">
-      <c r="A20" s="62"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -20420,7 +20446,7 @@
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
-      <c r="J20" s="70"/>
+      <c r="J20" s="72"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
       <c r="M20" s="16"/>
@@ -20429,10 +20455,10 @@
       <c r="P20" s="16"/>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
-      <c r="S20" s="61"/>
+      <c r="S20" s="63"/>
     </row>
     <row r="21">
-      <c r="A21" s="62"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -20441,7 +20467,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
-      <c r="J21" s="70"/>
+      <c r="J21" s="72"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
@@ -20450,10 +20476,10 @@
       <c r="P21" s="16"/>
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
-      <c r="S21" s="64"/>
+      <c r="S21" s="66"/>
     </row>
     <row r="22">
-      <c r="A22" s="62"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
@@ -20462,7 +20488,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="70"/>
+      <c r="J22" s="72"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
       <c r="M22" s="16"/>
@@ -20471,10 +20497,10 @@
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
-      <c r="S22" s="61"/>
+      <c r="S22" s="63"/>
     </row>
     <row r="23">
-      <c r="A23" s="62"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
@@ -20483,7 +20509,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
-      <c r="J23" s="70"/>
+      <c r="J23" s="72"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
       <c r="M23" s="16"/>
@@ -20492,10 +20518,10 @@
       <c r="P23" s="16"/>
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
-      <c r="S23" s="64"/>
+      <c r="S23" s="66"/>
     </row>
     <row r="24">
-      <c r="A24" s="62"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
@@ -20504,7 +20530,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
-      <c r="J24" s="70"/>
+      <c r="J24" s="72"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -20513,10 +20539,10 @@
       <c r="P24" s="16"/>
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
-      <c r="S24" s="61"/>
+      <c r="S24" s="63"/>
     </row>
     <row r="25">
-      <c r="A25" s="62"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
@@ -20525,7 +20551,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
-      <c r="J25" s="70"/>
+      <c r="J25" s="72"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
@@ -20534,10 +20560,10 @@
       <c r="P25" s="16"/>
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
-      <c r="S25" s="64"/>
+      <c r="S25" s="66"/>
     </row>
     <row r="26">
-      <c r="A26" s="62"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
@@ -20546,7 +20572,7 @@
       <c r="G26" s="16"/>
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
-      <c r="J26" s="70"/>
+      <c r="J26" s="72"/>
       <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
@@ -20555,10 +20581,10 @@
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
-      <c r="S26" s="61"/>
+      <c r="S26" s="63"/>
     </row>
     <row r="27">
-      <c r="A27" s="62"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16"/>
@@ -20567,7 +20593,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
-      <c r="J27" s="70"/>
+      <c r="J27" s="72"/>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
@@ -20576,10 +20602,10 @@
       <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
-      <c r="S27" s="64"/>
+      <c r="S27" s="66"/>
     </row>
     <row r="28">
-      <c r="A28" s="62"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="16"/>
@@ -20588,7 +20614,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
-      <c r="J28" s="70"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="16"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
@@ -20597,70 +20623,70 @@
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
-      <c r="S28" s="61"/>
+      <c r="S28" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:I6"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="R12:R13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="J6:J7"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="R10:R11"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="J10:J11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="J12:J13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="O16:O17"/>
     <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="R16:R17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
   </mergeCells>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" sqref="N8">
@@ -20694,181 +20720,181 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="71" t="s">
+      <c r="B1" s="73" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="71" t="s">
-        <v>203</v>
-      </c>
-      <c r="G1" s="71" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="71" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="71" t="s">
+      <c r="F1" s="73" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" s="73" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="K1" s="71" t="s">
-        <v>207</v>
-      </c>
-      <c r="M1" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" s="71" t="s">
-        <v>135</v>
+      <c r="J1" s="73" t="s">
+        <v>210</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>211</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="71" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" s="71" t="s">
+      <c r="B2" s="73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>213</v>
+      </c>
+      <c r="D2" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="71" t="s">
-        <v>210</v>
-      </c>
-      <c r="I2" s="71" t="s">
+      <c r="F2" s="73" t="s">
+        <v>214</v>
+      </c>
+      <c r="I2" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="71" t="s">
+      <c r="K2" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="71" t="s">
-        <v>211</v>
-      </c>
-      <c r="N2" s="71" t="s">
-        <v>212</v>
+      <c r="M2" s="73" t="s">
+        <v>215</v>
+      </c>
+      <c r="N2" s="73" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="71" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="71" t="s">
-        <v>214</v>
-      </c>
-      <c r="C3" s="71" t="s">
+      <c r="A3" s="73" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="71" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" s="71" t="s">
-        <v>216</v>
-      </c>
-      <c r="I3" s="71" t="s">
+      <c r="E3" s="73" t="s">
+        <v>219</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>220</v>
+      </c>
+      <c r="I3" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="71" t="s">
-        <v>217</v>
-      </c>
-      <c r="M3" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="N3" s="71" t="s">
-        <v>218</v>
+      <c r="K3" s="73" t="s">
+        <v>221</v>
+      </c>
+      <c r="M3" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="N3" s="73" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="71" t="e">
+      <c r="A4" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="B4" s="71" t="s">
-        <v>219</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>220</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="71" t="s">
+      <c r="B4" s="73" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="71" t="s">
-        <v>222</v>
-      </c>
-      <c r="I4" s="71" t="e">
+      <c r="F4" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="I4" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="K4" s="71" t="s">
+      <c r="K4" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="71" t="s">
-        <v>223</v>
-      </c>
-      <c r="N4" s="71" t="s">
-        <v>146</v>
+      <c r="M4" s="73" t="s">
+        <v>227</v>
+      </c>
+      <c r="N4" s="73" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="71" t="s">
-        <v>224</v>
-      </c>
-      <c r="C5" s="71" t="e">
+      <c r="B5" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D5" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="71" t="e">
+      <c r="D5" s="73" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="F5" s="71" t="s">
-        <v>226</v>
-      </c>
-      <c r="K5" s="71" t="e">
+      <c r="F5" s="73" t="s">
+        <v>230</v>
+      </c>
+      <c r="K5" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M5" s="71" t="s">
-        <v>227</v>
+      <c r="M5" s="73" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="71" t="s">
-        <v>228</v>
-      </c>
-      <c r="D6" s="71" t="s">
-        <v>229</v>
-      </c>
-      <c r="F6" s="71" t="e">
+      <c r="B6" s="73" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="73" t="e">
         <v>#N/A</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="71" t="e">
+      <c r="B7" s="73" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D7" s="71" t="e">
+      <c r="D7" s="73" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>